<commit_message>
Mise à jour du fichier Excel via Shiny
</commit_message>
<xml_diff>
--- a/VA_result_AEX.xlsx
+++ b/VA_result_AEX.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t xml:space="preserve">time</t>
   </si>
@@ -390,6 +390,54 @@
   </si>
   <si>
     <t xml:space="preserve">2025-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026-07-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2026-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2027-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2027-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2027-07-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2027-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2028-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2028-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2028-07-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2028-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2029-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2029-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2029-07-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2029-10-01</t>
   </si>
   <si>
     <t xml:space="preserve">VA_CST</t>
@@ -568,7 +616,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500"/>
+        <fgColor rgb="FFB8F0F6"/>
       </patternFill>
     </fill>
   </fills>
@@ -2433,6 +2481,182 @@
         <v>113.928136614758</v>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>124</v>
+      </c>
+      <c r="B122" t="n">
+        <v>1474101.0200077</v>
+      </c>
+      <c r="C122" t="n">
+        <v>147.41010200077</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>125</v>
+      </c>
+      <c r="B123" t="n">
+        <v>1546641.44983486</v>
+      </c>
+      <c r="C123" t="n">
+        <v>154.664144983486</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>126</v>
+      </c>
+      <c r="B124" t="n">
+        <v>1201882.2684693</v>
+      </c>
+      <c r="C124" t="n">
+        <v>120.18822684693</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125" t="n">
+        <v>1164991.82909282</v>
+      </c>
+      <c r="C125" t="n">
+        <v>116.499182909282</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>128</v>
+      </c>
+      <c r="B126" t="n">
+        <v>1490278.62799747</v>
+      </c>
+      <c r="C126" t="n">
+        <v>149.027862799747</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>129</v>
+      </c>
+      <c r="B127" t="n">
+        <v>1562220.55493122</v>
+      </c>
+      <c r="C127" t="n">
+        <v>156.222055493122</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>130</v>
+      </c>
+      <c r="B128" t="n">
+        <v>1219478.2545324</v>
+      </c>
+      <c r="C128" t="n">
+        <v>121.94782545324</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>131</v>
+      </c>
+      <c r="B129" t="n">
+        <v>1182707.75122326</v>
+      </c>
+      <c r="C129" t="n">
+        <v>118.270775122326</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>132</v>
+      </c>
+      <c r="B130" t="n">
+        <v>1514418.64975171</v>
+      </c>
+      <c r="C130" t="n">
+        <v>151.441864975171</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>133</v>
+      </c>
+      <c r="B131" t="n">
+        <v>1588812.5967412</v>
+      </c>
+      <c r="C131" t="n">
+        <v>158.88125967412</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>134</v>
+      </c>
+      <c r="B132" t="n">
+        <v>1242886.39542261</v>
+      </c>
+      <c r="C132" t="n">
+        <v>124.288639542261</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>135</v>
+      </c>
+      <c r="B133" t="n">
+        <v>1206938.63978257</v>
+      </c>
+      <c r="C133" t="n">
+        <v>120.693863978257</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>136</v>
+      </c>
+      <c r="B134" t="n">
+        <v>1537720.63381413</v>
+      </c>
+      <c r="C134" t="n">
+        <v>153.772063381413</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>137</v>
+      </c>
+      <c r="B135" t="n">
+        <v>1610026.22872905</v>
+      </c>
+      <c r="C135" t="n">
+        <v>161.002622872905</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>138</v>
+      </c>
+      <c r="B136" t="n">
+        <v>1266067.16133615</v>
+      </c>
+      <c r="C136" t="n">
+        <v>126.606716133615</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>139</v>
+      </c>
+      <c r="B137" t="n">
+        <v>1229229.73251363</v>
+      </c>
+      <c r="C137" t="n">
+        <v>122.922973251363</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2452,19 +2676,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2">
@@ -2498,7 +2722,7 @@
         <v>16.8587441874193</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4">
@@ -2518,7 +2742,7 @@
         <v>11.4186726092878</v>
       </c>
       <c r="F4" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5">
@@ -2538,7 +2762,7 @@
         <v>-32.240621440938</v>
       </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6">
@@ -2558,7 +2782,7 @@
         <v>37.9695690633087</v>
       </c>
       <c r="F6" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7">
@@ -2578,7 +2802,7 @@
         <v>-7.43415870797737</v>
       </c>
       <c r="F7" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8">
@@ -2598,7 +2822,7 @@
         <v>-5.1376532541995</v>
       </c>
       <c r="F8" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9">
@@ -2618,7 +2842,7 @@
         <v>-4.54362263052331</v>
       </c>
       <c r="F9" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10">
@@ -2638,7 +2862,7 @@
         <v>-8.64330036119539</v>
       </c>
       <c r="F10" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11">
@@ -2658,7 +2882,7 @@
         <v>-2.63607280820545</v>
       </c>
       <c r="F11" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12">
@@ -2678,7 +2902,7 @@
         <v>23.6030197825734</v>
       </c>
       <c r="F12" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13">
@@ -2698,7 +2922,7 @@
         <v>-1.06245501423519</v>
       </c>
       <c r="F13" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14">
@@ -2718,7 +2942,7 @@
         <v>-11.4626085429733</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15">
@@ -2738,7 +2962,7 @@
         <v>13.3018769661764</v>
       </c>
       <c r="F15" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16">
@@ -2758,7 +2982,7 @@
         <v>1.3543587726772</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17">
@@ -2778,7 +3002,7 @@
         <v>11.1818584973771</v>
       </c>
       <c r="F17" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18">
@@ -2798,7 +3022,7 @@
         <v>4.95685158499166</v>
       </c>
       <c r="F18" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19">
@@ -2818,7 +3042,7 @@
         <v>7.64736356794891</v>
       </c>
       <c r="F19" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20">
@@ -2838,7 +3062,7 @@
         <v>2.94659925481584</v>
       </c>
       <c r="F20" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21">
@@ -2858,7 +3082,7 @@
         <v>11.7969596475774</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22">
@@ -2878,7 +3102,7 @@
         <v>-9.37199005076323</v>
       </c>
       <c r="F22" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23">
@@ -2898,7 +3122,7 @@
         <v>17.7644571880596</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24">
@@ -2918,7 +3142,7 @@
         <v>6.45262473971155</v>
       </c>
       <c r="F24" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25">
@@ -2938,7 +3162,7 @@
         <v>0.484550598724365</v>
       </c>
       <c r="F25" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26">
@@ -2958,7 +3182,7 @@
         <v>6.30588032849637</v>
       </c>
       <c r="F26" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27">
@@ -2972,13 +3196,13 @@
         <v>122.923892886888</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.600002038385694</v>
+        <v>-0.600002038385705</v>
       </c>
       <c r="E27" t="n">
         <v>1.28535867435131</v>
       </c>
       <c r="F27" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28">
@@ -2986,19 +3210,19 @@
         <v>108</v>
       </c>
       <c r="B28" t="n">
-        <v>3618641.92120793</v>
+        <v>3579204.4350852</v>
       </c>
       <c r="C28" t="n">
         <v>124.508997220763</v>
       </c>
       <c r="D28" t="n">
-        <v>0.66641001096801</v>
+        <v>-0.430694989823976</v>
       </c>
       <c r="E28" t="n">
         <v>1.2895005980111</v>
       </c>
       <c r="F28" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29">
@@ -3006,19 +3230,19 @@
         <v>112</v>
       </c>
       <c r="B29" t="n">
-        <v>3677921.38954705</v>
+        <v>3604130.19693149</v>
       </c>
       <c r="C29" t="n">
         <v>128.43146704908</v>
       </c>
       <c r="D29" t="n">
-        <v>1.63816894928726</v>
+        <v>0.696405089409136</v>
       </c>
       <c r="E29" t="n">
         <v>3.15035050949972</v>
       </c>
       <c r="F29" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30">
@@ -3026,19 +3250,19 @@
         <v>116</v>
       </c>
       <c r="B30" t="n">
-        <v>3696343.06674467</v>
+        <v>3592626.61098929</v>
       </c>
       <c r="C30" t="n">
         <v>129.650413085864</v>
       </c>
       <c r="D30" t="n">
-        <v>0.50087196670292</v>
+        <v>-0.319177868546294</v>
       </c>
       <c r="E30" t="n">
         <v>0.949102322656037</v>
       </c>
       <c r="F30" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31">
@@ -3046,19 +3270,99 @@
         <v>120</v>
       </c>
       <c r="B31" t="n">
-        <v>3732002.87844862</v>
+        <v>3602218.74425587</v>
       </c>
       <c r="C31" t="n">
         <v>132.009991189569</v>
       </c>
       <c r="D31" t="n">
-        <v>0.964732197743778</v>
+        <v>0.266994995729308</v>
       </c>
       <c r="E31" t="n">
         <v>1.81995417333685</v>
       </c>
       <c r="F31" t="s">
-        <v>129</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" t="n">
+        <v>3620020.05334474</v>
+      </c>
+      <c r="C32" t="n">
+        <v>134.690414185117</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.494176238387767</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.0304697935315</v>
+      </c>
+      <c r="F32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" t="n">
+        <v>3625579.68582084</v>
+      </c>
+      <c r="C33" t="n">
+        <v>136.367129717109</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.153580156854782</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1.24486626768225</v>
+      </c>
+      <c r="F33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" t="n">
+        <v>3645515.82603915</v>
+      </c>
+      <c r="C34" t="n">
+        <v>138.826407042452</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.549874556509544</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.80342383860777</v>
+      </c>
+      <c r="F34" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" t="n">
+        <v>3664505.59427553</v>
+      </c>
+      <c r="C35" t="n">
+        <v>141.076093909824</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.5209075791345</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.62050355930035</v>
+      </c>
+      <c r="F35" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3080,19 +3384,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2">
@@ -3594,34 +3898,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2">
@@ -3656,7 +3960,7 @@
         <v>2471528.25793099</v>
       </c>
       <c r="K2" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3">
@@ -3691,7 +3995,7 @@
         <v>2471528.25793099</v>
       </c>
       <c r="K3" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4">
@@ -3726,7 +4030,7 @@
         <v>2471528.25793099</v>
       </c>
       <c r="K4" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5">
@@ -3761,7 +4065,7 @@
         <v>2471528.25793099</v>
       </c>
       <c r="K5" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6">
@@ -3796,7 +4100,7 @@
         <v>2752196.12152272</v>
       </c>
       <c r="K6" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7">
@@ -3831,7 +4135,7 @@
         <v>2752196.12152272</v>
       </c>
       <c r="K7" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8">
@@ -3866,7 +4170,7 @@
         <v>2752196.12152272</v>
       </c>
       <c r="K8" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9">
@@ -3901,7 +4205,7 @@
         <v>2752196.12152272</v>
       </c>
       <c r="K9" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10">
@@ -3936,7 +4240,7 @@
         <v>2425737.21499481</v>
       </c>
       <c r="K10" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11">
@@ -3971,7 +4275,7 @@
         <v>2425737.21499481</v>
       </c>
       <c r="K11" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12">
@@ -4006,7 +4310,7 @@
         <v>2425737.21499481</v>
       </c>
       <c r="K12" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13">
@@ -4041,7 +4345,7 @@
         <v>2425737.21499481</v>
       </c>
       <c r="K13" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14">
@@ -4076,7 +4380,7 @@
         <v>2491235.53626033</v>
       </c>
       <c r="K14" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15">
@@ -4111,7 +4415,7 @@
         <v>2491235.53626033</v>
       </c>
       <c r="K15" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16">
@@ -4146,7 +4450,7 @@
         <v>2491235.53626033</v>
       </c>
       <c r="K16" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17">
@@ -4181,7 +4485,7 @@
         <v>2491235.53626033</v>
       </c>
       <c r="K17" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18">
@@ -4216,7 +4520,7 @@
         <v>2222014.48918456</v>
       </c>
       <c r="K18" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19">
@@ -4251,7 +4555,7 @@
         <v>2222014.48918456</v>
       </c>
       <c r="K19" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20">
@@ -4286,7 +4590,7 @@
         <v>2222014.48918456</v>
       </c>
       <c r="K20" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
@@ -4321,7 +4625,7 @@
         <v>2222014.48918456</v>
       </c>
       <c r="K21" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22">
@@ -4356,7 +4660,7 @@
         <v>2147633.16721365</v>
       </c>
       <c r="K22" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23">
@@ -4391,7 +4695,7 @@
         <v>2147633.16721365</v>
       </c>
       <c r="K23" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24">
@@ -4426,7 +4730,7 @@
         <v>2147633.16721365</v>
       </c>
       <c r="K24" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25">
@@ -4461,7 +4765,7 @@
         <v>2147633.16721365</v>
       </c>
       <c r="K25" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26">
@@ -4496,7 +4800,7 @@
         <v>2144690.37194562</v>
       </c>
       <c r="K26" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27">
@@ -4531,7 +4835,7 @@
         <v>2144690.37194562</v>
       </c>
       <c r="K27" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28">
@@ -4566,7 +4870,7 @@
         <v>2144690.37194562</v>
       </c>
       <c r="K28" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29">
@@ -4601,7 +4905,7 @@
         <v>2144690.37194562</v>
       </c>
       <c r="K29" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30">
@@ -4636,7 +4940,7 @@
         <v>1961631.27389447</v>
       </c>
       <c r="K30" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31">
@@ -4671,7 +4975,7 @@
         <v>1961631.27389447</v>
       </c>
       <c r="K31" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32">
@@ -4706,7 +5010,7 @@
         <v>1961631.27389447</v>
       </c>
       <c r="K32" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33">
@@ -4741,7 +5045,7 @@
         <v>1961631.27389447</v>
       </c>
       <c r="K33" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34">
@@ -4776,7 +5080,7 @@
         <v>1912882.39766133</v>
       </c>
       <c r="K34" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35">
@@ -4811,7 +5115,7 @@
         <v>1912882.39766133</v>
       </c>
       <c r="K35" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36">
@@ -4846,7 +5150,7 @@
         <v>1912882.39766133</v>
       </c>
       <c r="K36" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37">
@@ -4881,7 +5185,7 @@
         <v>1912882.39766133</v>
       </c>
       <c r="K37" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38">
@@ -4916,7 +5220,7 @@
         <v>2111466.31439091</v>
       </c>
       <c r="K38" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39">
@@ -4951,7 +5255,7 @@
         <v>2111466.31439091</v>
       </c>
       <c r="K39" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40">
@@ -4986,7 +5290,7 @@
         <v>2111466.31439091</v>
       </c>
       <c r="K40" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41">
@@ -5021,7 +5325,7 @@
         <v>2111466.31439091</v>
       </c>
       <c r="K41" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42">
@@ -5056,7 +5360,7 @@
         <v>1970376.85213617</v>
       </c>
       <c r="K42" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43">
@@ -5091,7 +5395,7 @@
         <v>1970376.85213617</v>
       </c>
       <c r="K43" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44">
@@ -5126,7 +5430,7 @@
         <v>1970376.85213617</v>
       </c>
       <c r="K44" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45">
@@ -5161,7 +5465,7 @@
         <v>1970376.85213617</v>
       </c>
       <c r="K45" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46">
@@ -5196,7 +5500,7 @@
         <v>1914995.21927437</v>
       </c>
       <c r="K46" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47">
@@ -5231,7 +5535,7 @@
         <v>1914995.21927437</v>
       </c>
       <c r="K47" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48">
@@ -5266,7 +5570,7 @@
         <v>1914995.21927437</v>
       </c>
       <c r="K48" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49">
@@ -5301,7 +5605,7 @@
         <v>1914995.21927437</v>
       </c>
       <c r="K49" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50">
@@ -5336,7 +5640,7 @@
         <v>1987364.03083003</v>
       </c>
       <c r="K50" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51">
@@ -5371,7 +5675,7 @@
         <v>1987364.03083003</v>
       </c>
       <c r="K51" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52">
@@ -5406,7 +5710,7 @@
         <v>1987364.03083003</v>
       </c>
       <c r="K52" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
     </row>
     <row r="53">
@@ -5441,7 +5745,7 @@
         <v>1987364.03083003</v>
       </c>
       <c r="K53" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54">
@@ -5476,7 +5780,7 @@
         <v>2133815.29888369</v>
       </c>
       <c r="K54" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55">
@@ -5511,7 +5815,7 @@
         <v>2133815.29888369</v>
       </c>
       <c r="K55" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56">
@@ -5546,7 +5850,7 @@
         <v>2133815.29888369</v>
       </c>
       <c r="K56" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57">
@@ -5581,7 +5885,7 @@
         <v>2133815.29888369</v>
       </c>
       <c r="K57" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58">
@@ -5616,7 +5920,7 @@
         <v>2303811.56475951</v>
       </c>
       <c r="K58" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59">
@@ -5651,7 +5955,7 @@
         <v>2303811.56475951</v>
       </c>
       <c r="K59" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60">
@@ -5686,7 +5990,7 @@
         <v>2303811.56475951</v>
       </c>
       <c r="K60" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61">
@@ -5721,7 +6025,7 @@
         <v>2303811.56475951</v>
       </c>
       <c r="K61" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62">
@@ -5756,7 +6060,7 @@
         <v>2417541.6126855</v>
       </c>
       <c r="K62" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63">
@@ -5791,7 +6095,7 @@
         <v>2417541.6126855</v>
       </c>
       <c r="K63" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64">
@@ -5826,7 +6130,7 @@
         <v>2417541.6126855</v>
       </c>
       <c r="K64" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65">
@@ -5861,7 +6165,7 @@
         <v>2417541.6126855</v>
       </c>
       <c r="K65" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66">
@@ -5896,7 +6200,7 @@
         <v>2723723.35787271</v>
       </c>
       <c r="K66" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67">
@@ -5931,7 +6235,7 @@
         <v>2723723.35787271</v>
       </c>
       <c r="K67" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68">
@@ -5966,7 +6270,7 @@
         <v>2723723.35787271</v>
       </c>
       <c r="K68" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69">
@@ -6001,7 +6305,7 @@
         <v>2723723.35787271</v>
       </c>
       <c r="K69" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70">
@@ -6036,7 +6340,7 @@
         <v>3128364.70384383</v>
       </c>
       <c r="K70" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="71">
@@ -6071,7 +6375,7 @@
         <v>3128364.70384383</v>
       </c>
       <c r="K71" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72">
@@ -6106,7 +6410,7 @@
         <v>3128364.70384383</v>
       </c>
       <c r="K72" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="73">
@@ -6141,7 +6445,7 @@
         <v>3128364.70384383</v>
       </c>
       <c r="K73" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74">
@@ -6176,7 +6480,7 @@
         <v>3274593.17477957</v>
       </c>
       <c r="K74" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75">
@@ -6211,7 +6515,7 @@
         <v>3274593.17477957</v>
       </c>
       <c r="K75" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="76">
@@ -6246,7 +6550,7 @@
         <v>3274593.17477957</v>
       </c>
       <c r="K76" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77">
@@ -6281,7 +6585,7 @@
         <v>3274593.17477957</v>
       </c>
       <c r="K77" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78">
@@ -6316,7 +6620,7 @@
         <v>3055286.16569364</v>
       </c>
       <c r="K78" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79">
@@ -6351,7 +6655,7 @@
         <v>3055286.16569364</v>
       </c>
       <c r="K79" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
     </row>
     <row r="80">
@@ -6386,7 +6690,7 @@
         <v>3055286.16569364</v>
       </c>
       <c r="K80" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81">
@@ -6421,7 +6725,7 @@
         <v>3055286.16569364</v>
       </c>
       <c r="K81" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82">
@@ -6456,7 +6760,7 @@
         <v>3053589.51327894</v>
       </c>
       <c r="K82" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83">
@@ -6491,7 +6795,7 @@
         <v>3053589.51327894</v>
       </c>
       <c r="K83" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84">
@@ -6526,7 +6830,7 @@
         <v>3053589.51327894</v>
       </c>
       <c r="K84" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
     </row>
     <row r="85">
@@ -6561,7 +6865,7 @@
         <v>3053589.51327894</v>
       </c>
       <c r="K85" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
     </row>
     <row r="86">
@@ -6596,7 +6900,7 @@
         <v>3314032.27574181</v>
       </c>
       <c r="K86" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87">
@@ -6631,7 +6935,7 @@
         <v>3314032.27574181</v>
       </c>
       <c r="K87" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
     </row>
     <row r="88">
@@ -6666,7 +6970,7 @@
         <v>3314032.27574181</v>
       </c>
       <c r="K88" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
     </row>
     <row r="89">
@@ -6701,7 +7005,7 @@
         <v>3314032.27574181</v>
       </c>
       <c r="K89" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
     </row>
     <row r="90">
@@ -6736,7 +7040,7 @@
         <v>3509548.69777691</v>
       </c>
       <c r="K90" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="91">
@@ -6771,7 +7075,7 @@
         <v>3509548.69777691</v>
       </c>
       <c r="K91" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="92">
@@ -6806,7 +7110,7 @@
         <v>3509548.69777691</v>
       </c>
       <c r="K92" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="93">
@@ -6841,7 +7145,7 @@
         <v>3509548.69777691</v>
       </c>
       <c r="K93" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
     </row>
     <row r="94">
@@ -6876,7 +7180,7 @@
         <v>3616384.953479</v>
       </c>
       <c r="K94" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="95">
@@ -6911,7 +7215,7 @@
         <v>3616384.953479</v>
       </c>
       <c r="K95" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="96">
@@ -6946,7 +7250,7 @@
         <v>3616384.953479</v>
       </c>
       <c r="K96" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
     </row>
     <row r="97">
@@ -6981,7 +7285,7 @@
         <v>3616384.953479</v>
       </c>
       <c r="K97" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -7003,13 +7307,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2">
@@ -8361,13 +8665,13 @@
         <v>104</v>
       </c>
       <c r="B98" t="n">
-        <v>947127.35240704</v>
+        <v>949087.193975166</v>
       </c>
       <c r="C98" t="n">
         <v>33.9372445565342</v>
       </c>
       <c r="D98" t="n">
-        <v>351210.388774885</v>
+        <v>90052.4628570333</v>
       </c>
     </row>
     <row r="99">
@@ -8375,13 +8679,13 @@
         <v>105</v>
       </c>
       <c r="B99" t="n">
-        <v>971660.060284155</v>
+        <v>972835.96522503</v>
       </c>
       <c r="C99" t="n">
         <v>35.560552071784</v>
       </c>
       <c r="D99" t="n">
-        <v>351210.388774885</v>
+        <v>89152.5165917085</v>
       </c>
     </row>
     <row r="100">
@@ -8389,13 +8693,13 @@
         <v>106</v>
       </c>
       <c r="B100" t="n">
-        <v>845397.045395155</v>
+        <v>845005.07708153</v>
       </c>
       <c r="C100" t="n">
         <v>27.2058403948636</v>
       </c>
       <c r="D100" t="n">
-        <v>351210.388774885</v>
+        <v>87352.6240610589</v>
       </c>
     </row>
     <row r="101">
@@ -8403,13 +8707,13 @@
         <v>107</v>
       </c>
       <c r="B101" t="n">
-        <v>830502.111955899</v>
+        <v>827758.333760523</v>
       </c>
       <c r="C101" t="n">
         <v>26.2202558637061</v>
       </c>
       <c r="D101" t="n">
-        <v>351210.388774885</v>
+        <v>84652.7852650844</v>
       </c>
     </row>
     <row r="102">
@@ -8417,13 +8721,13 @@
         <v>108</v>
       </c>
       <c r="B102" t="n">
-        <v>951197.065312656</v>
+        <v>945317.540608278</v>
       </c>
       <c r="C102" t="n">
         <v>34.2065338489224</v>
       </c>
       <c r="D102" t="n">
-        <v>351210.388774885</v>
+        <v>81053.0002037852</v>
       </c>
     </row>
     <row r="103">
@@ -8431,13 +8735,13 @@
         <v>109</v>
       </c>
       <c r="B103" t="n">
-        <v>980471.960178461</v>
+        <v>971746.198139961</v>
       </c>
       <c r="C103" t="n">
         <v>36.1436276700305</v>
       </c>
       <c r="D103" t="n">
-        <v>351210.388774885</v>
+        <v>77785.566880691</v>
       </c>
     </row>
     <row r="104">
@@ -8445,13 +8749,13 @@
         <v>110</v>
       </c>
       <c r="B104" t="n">
-        <v>849889.323955543</v>
+        <v>838606.833757799</v>
       </c>
       <c r="C104" t="n">
         <v>27.5030904817354</v>
       </c>
       <c r="D104" t="n">
-        <v>351210.388774885</v>
+        <v>74850.4852958017</v>
       </c>
     </row>
     <row r="105">
@@ -8459,13 +8763,13 @@
         <v>111</v>
       </c>
       <c r="B105" t="n">
-        <v>837083.571761274</v>
+        <v>823533.862579164</v>
       </c>
       <c r="C105" t="n">
         <v>26.6557452200745</v>
       </c>
       <c r="D105" t="n">
-        <v>351210.388774885</v>
+        <v>72247.7554491175</v>
       </c>
     </row>
     <row r="106">
@@ -8473,13 +8777,13 @@
         <v>112</v>
       </c>
       <c r="B106" t="n">
-        <v>967345.226152594</v>
+        <v>951817.807160997</v>
       </c>
       <c r="C106" t="n">
         <v>35.2750433253422</v>
       </c>
       <c r="D106" t="n">
-        <v>351210.388774885</v>
+        <v>69977.3773406383</v>
       </c>
     </row>
     <row r="107">
@@ -8487,13 +8791,13 @@
         <v>113</v>
       </c>
       <c r="B107" t="n">
-        <v>995787.077341421</v>
+        <v>978300.422761112</v>
       </c>
       <c r="C107" t="n">
         <v>37.157015385406</v>
       </c>
       <c r="D107" t="n">
-        <v>351210.388774885</v>
+        <v>67728.2073316577</v>
       </c>
     </row>
     <row r="108">
@@ -8501,13 +8805,13 @@
         <v>114</v>
       </c>
       <c r="B108" t="n">
-        <v>864196.473857754</v>
+        <v>844769.057909508</v>
       </c>
       <c r="C108" t="n">
         <v>28.4497818977177</v>
       </c>
       <c r="D108" t="n">
-        <v>351210.388774885</v>
+        <v>65500.2454221755</v>
       </c>
     </row>
     <row r="109">
@@ -8515,13 +8819,13 @@
         <v>115</v>
       </c>
       <c r="B109" t="n">
-        <v>850592.612195284</v>
+        <v>829242.909099876</v>
       </c>
       <c r="C109" t="n">
         <v>27.5496264406144</v>
       </c>
       <c r="D109" t="n">
-        <v>351210.388774885</v>
+        <v>63293.491612192</v>
       </c>
     </row>
     <row r="110">
@@ -8529,13 +8833,13 @@
         <v>116</v>
       </c>
       <c r="B110" t="n">
-        <v>972201.267078259</v>
+        <v>948947.751056463</v>
       </c>
       <c r="C110" t="n">
         <v>35.5963632452009</v>
       </c>
       <c r="D110" t="n">
-        <v>351210.388774885</v>
+        <v>61107.9459017069</v>
       </c>
     </row>
     <row r="111">
@@ -8543,13 +8847,13 @@
         <v>117</v>
       </c>
       <c r="B111" t="n">
-        <v>998340.223403716</v>
+        <v>973254.943044547</v>
       </c>
       <c r="C111" t="n">
         <v>37.3259547952427</v>
       </c>
       <c r="D111" t="n">
-        <v>351210.388774885</v>
+        <v>59005.1107782136</v>
       </c>
     </row>
     <row r="112">
@@ -8557,13 +8861,13 @@
         <v>118</v>
       </c>
       <c r="B112" t="n">
-        <v>870045.07346231</v>
+        <v>843200.07735478</v>
       </c>
       <c r="C112" t="n">
         <v>28.8367785447783</v>
       </c>
       <c r="D112" t="n">
-        <v>351210.388774885</v>
+        <v>56984.986241712</v>
       </c>
     </row>
     <row r="113">
@@ -8571,13 +8875,13 @@
         <v>119</v>
       </c>
       <c r="B113" t="n">
-        <v>855756.502800381</v>
+        <v>827223.839533503</v>
       </c>
       <c r="C113" t="n">
         <v>27.8913165006424</v>
       </c>
       <c r="D113" t="n">
-        <v>351210.388774885</v>
+        <v>55047.5722922022</v>
       </c>
     </row>
     <row r="114">
@@ -8585,13 +8889,13 @@
         <v>120</v>
       </c>
       <c r="B114" t="n">
-        <v>980331.646378599</v>
+        <v>950183.364541386</v>
       </c>
       <c r="C114" t="n">
         <v>36.1343432303775</v>
       </c>
       <c r="D114" t="n">
-        <v>351210.388774885</v>
+        <v>53192.8689296841</v>
       </c>
     </row>
     <row r="115">
@@ -8599,13 +8903,13 @@
         <v>121</v>
       </c>
       <c r="B115" t="n">
-        <v>1009013.89467784</v>
+        <v>977300.264728106</v>
       </c>
       <c r="C115" t="n">
         <v>38.0322221539617</v>
       </c>
       <c r="D115" t="n">
-        <v>351210.388774885</v>
+        <v>51395.8752202055</v>
       </c>
     </row>
     <row r="116">
@@ -8613,13 +8917,13 @@
         <v>122</v>
       </c>
       <c r="B116" t="n">
-        <v>877973.441917326</v>
+        <v>844744.734312878</v>
       </c>
       <c r="C116" t="n">
         <v>29.3613916515403</v>
       </c>
       <c r="D116" t="n">
-        <v>351210.388774885</v>
+        <v>49656.5911637664</v>
       </c>
     </row>
     <row r="117">
@@ -8627,13 +8931,237 @@
         <v>123</v>
       </c>
       <c r="B117" t="n">
-        <v>864683.895474854</v>
+        <v>829990.380673505</v>
       </c>
       <c r="C117" t="n">
         <v>28.4820341536894</v>
       </c>
       <c r="D117" t="n">
-        <v>351210.388774885</v>
+        <v>47975.0167603667</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>124</v>
+      </c>
+      <c r="B118" t="n">
+        <v>955077.333678383</v>
+      </c>
+      <c r="C118" t="n">
+        <v>36.8525255001924</v>
+      </c>
+      <c r="D118" t="n">
+        <v>46351.1520100066</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>125</v>
+      </c>
+      <c r="B119" t="n">
+        <v>981112.799350174</v>
+      </c>
+      <c r="C119" t="n">
+        <v>38.6660362458715</v>
+      </c>
+      <c r="D119" t="n">
+        <v>44776.4126695248</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>126</v>
+      </c>
+      <c r="B120" t="n">
+        <v>849527.008291201</v>
+      </c>
+      <c r="C120" t="n">
+        <v>30.0470567117325</v>
+      </c>
+      <c r="D120" t="n">
+        <v>43250.7987389214</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>127</v>
+      </c>
+      <c r="B121" t="n">
+        <v>834302.912024979</v>
+      </c>
+      <c r="C121" t="n">
+        <v>29.1247957273204</v>
+      </c>
+      <c r="D121" t="n">
+        <v>41774.3102181964</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>128</v>
+      </c>
+      <c r="B122" t="n">
+        <v>955959.334961889</v>
+      </c>
+      <c r="C122" t="n">
+        <v>37.2569656999367</v>
+      </c>
+      <c r="D122" t="n">
+        <v>40346.9471073498</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>129</v>
+      </c>
+      <c r="B123" t="n">
+        <v>981951.208532833</v>
+      </c>
+      <c r="C123" t="n">
+        <v>39.0555138732806</v>
+      </c>
+      <c r="D123" t="n">
+        <v>38981.7539295919</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>130</v>
+      </c>
+      <c r="B124" t="n">
+        <v>851321.332130614</v>
+      </c>
+      <c r="C124" t="n">
+        <v>30.48695636331</v>
+      </c>
+      <c r="D124" t="n">
+        <v>37678.7306849226</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>131</v>
+      </c>
+      <c r="B125" t="n">
+        <v>836347.810195502</v>
+      </c>
+      <c r="C125" t="n">
+        <v>29.5676937805815</v>
+      </c>
+      <c r="D125" t="n">
+        <v>36437.8773733419</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>132</v>
+      </c>
+      <c r="B126" t="n">
+        <v>960648.008174092</v>
+      </c>
+      <c r="C126" t="n">
+        <v>37.8604662437928</v>
+      </c>
+      <c r="D126" t="n">
+        <v>35259.1939948499</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>133</v>
+      </c>
+      <c r="B127" t="n">
+        <v>987702.674023728</v>
+      </c>
+      <c r="C127" t="n">
+        <v>39.7203149185301</v>
+      </c>
+      <c r="D127" t="n">
+        <v>34050.5519932516</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>134</v>
+      </c>
+      <c r="B128" t="n">
+        <v>855925.974933839</v>
+      </c>
+      <c r="C128" t="n">
+        <v>31.0721598855652</v>
+      </c>
+      <c r="D128" t="n">
+        <v>32811.9513685472</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>135</v>
+      </c>
+      <c r="B129" t="n">
+        <v>841239.168907487</v>
+      </c>
+      <c r="C129" t="n">
+        <v>30.1734659945642</v>
+      </c>
+      <c r="D129" t="n">
+        <v>31543.3921207367</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>136</v>
+      </c>
+      <c r="B130" t="n">
+        <v>965084.02143623</v>
+      </c>
+      <c r="C130" t="n">
+        <v>38.4430158453531</v>
+      </c>
+      <c r="D130" t="n">
+        <v>30244.87424982</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>137</v>
+      </c>
+      <c r="B131" t="n">
+        <v>991554.158700586</v>
+      </c>
+      <c r="C131" t="n">
+        <v>40.2506557182263</v>
+      </c>
+      <c r="D131" t="n">
+        <v>29270.9858466324</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>138</v>
+      </c>
+      <c r="B132" t="n">
+        <v>861034.052974877</v>
+      </c>
+      <c r="C132" t="n">
+        <v>31.6516790334038</v>
+      </c>
+      <c r="D132" t="n">
+        <v>28621.7269111741</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>139</v>
+      </c>
+      <c r="B133" t="n">
+        <v>846833.361163838</v>
+      </c>
+      <c r="C133" t="n">
+        <v>30.7307433128408</v>
+      </c>
+      <c r="D133" t="n">
+        <v>28297.0974434449</v>
       </c>
     </row>
   </sheetData>
@@ -8655,7 +9183,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2">
@@ -9431,7 +9959,7 @@
         <v>104</v>
       </c>
       <c r="B98" t="n">
-        <v>947127.35240704</v>
+        <v>949087.193975166</v>
       </c>
     </row>
     <row r="99">
@@ -9439,7 +9967,7 @@
         <v>105</v>
       </c>
       <c r="B99" t="n">
-        <v>971660.060284155</v>
+        <v>972835.96522503</v>
       </c>
     </row>
     <row r="100">
@@ -9447,7 +9975,7 @@
         <v>106</v>
       </c>
       <c r="B100" t="n">
-        <v>845397.045395155</v>
+        <v>845005.07708153</v>
       </c>
     </row>
     <row r="101">
@@ -9455,7 +9983,7 @@
         <v>107</v>
       </c>
       <c r="B101" t="n">
-        <v>830502.111955899</v>
+        <v>827758.333760523</v>
       </c>
     </row>
     <row r="102">
@@ -9463,7 +9991,7 @@
         <v>108</v>
       </c>
       <c r="B102" t="n">
-        <v>951197.065312656</v>
+        <v>945317.540608278</v>
       </c>
     </row>
     <row r="103">
@@ -9471,7 +9999,7 @@
         <v>109</v>
       </c>
       <c r="B103" t="n">
-        <v>980471.960178461</v>
+        <v>971746.198139961</v>
       </c>
     </row>
     <row r="104">
@@ -9479,7 +10007,7 @@
         <v>110</v>
       </c>
       <c r="B104" t="n">
-        <v>849889.323955543</v>
+        <v>838606.833757799</v>
       </c>
     </row>
     <row r="105">
@@ -9487,7 +10015,7 @@
         <v>111</v>
       </c>
       <c r="B105" t="n">
-        <v>837083.571761274</v>
+        <v>823533.862579164</v>
       </c>
     </row>
     <row r="106">
@@ -9495,7 +10023,7 @@
         <v>112</v>
       </c>
       <c r="B106" t="n">
-        <v>967345.226152594</v>
+        <v>951817.807160997</v>
       </c>
     </row>
     <row r="107">
@@ -9503,7 +10031,7 @@
         <v>113</v>
       </c>
       <c r="B107" t="n">
-        <v>995787.077341421</v>
+        <v>978300.422761112</v>
       </c>
     </row>
     <row r="108">
@@ -9511,7 +10039,7 @@
         <v>114</v>
       </c>
       <c r="B108" t="n">
-        <v>864196.473857754</v>
+        <v>844769.057909508</v>
       </c>
     </row>
     <row r="109">
@@ -9519,7 +10047,7 @@
         <v>115</v>
       </c>
       <c r="B109" t="n">
-        <v>850592.612195284</v>
+        <v>829242.909099876</v>
       </c>
     </row>
     <row r="110">
@@ -9527,7 +10055,7 @@
         <v>116</v>
       </c>
       <c r="B110" t="n">
-        <v>972201.267078259</v>
+        <v>948947.751056463</v>
       </c>
     </row>
     <row r="111">
@@ -9535,7 +10063,7 @@
         <v>117</v>
       </c>
       <c r="B111" t="n">
-        <v>998340.223403716</v>
+        <v>973254.943044547</v>
       </c>
     </row>
     <row r="112">
@@ -9543,7 +10071,7 @@
         <v>118</v>
       </c>
       <c r="B112" t="n">
-        <v>870045.07346231</v>
+        <v>843200.07735478</v>
       </c>
     </row>
     <row r="113">
@@ -9551,7 +10079,7 @@
         <v>119</v>
       </c>
       <c r="B113" t="n">
-        <v>855756.502800381</v>
+        <v>827223.839533503</v>
       </c>
     </row>
     <row r="114">
@@ -9559,7 +10087,7 @@
         <v>120</v>
       </c>
       <c r="B114" t="n">
-        <v>980331.646378599</v>
+        <v>950183.364541386</v>
       </c>
     </row>
     <row r="115">
@@ -9567,7 +10095,7 @@
         <v>121</v>
       </c>
       <c r="B115" t="n">
-        <v>1009013.89467784</v>
+        <v>977300.264728106</v>
       </c>
     </row>
     <row r="116">
@@ -9575,7 +10103,7 @@
         <v>122</v>
       </c>
       <c r="B116" t="n">
-        <v>877973.441917326</v>
+        <v>844744.734312878</v>
       </c>
     </row>
     <row r="117">
@@ -9583,7 +10111,135 @@
         <v>123</v>
       </c>
       <c r="B117" t="n">
-        <v>864683.895474854</v>
+        <v>829990.380673505</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>124</v>
+      </c>
+      <c r="B118" t="n">
+        <v>955077.333678383</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>125</v>
+      </c>
+      <c r="B119" t="n">
+        <v>981112.799350174</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>126</v>
+      </c>
+      <c r="B120" t="n">
+        <v>849527.008291201</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>127</v>
+      </c>
+      <c r="B121" t="n">
+        <v>834302.912024979</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>128</v>
+      </c>
+      <c r="B122" t="n">
+        <v>955959.334961889</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>129</v>
+      </c>
+      <c r="B123" t="n">
+        <v>981951.208532833</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>130</v>
+      </c>
+      <c r="B124" t="n">
+        <v>851321.332130614</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>131</v>
+      </c>
+      <c r="B125" t="n">
+        <v>836347.810195502</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>132</v>
+      </c>
+      <c r="B126" t="n">
+        <v>960648.008174092</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>133</v>
+      </c>
+      <c r="B127" t="n">
+        <v>987702.674023728</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>134</v>
+      </c>
+      <c r="B128" t="n">
+        <v>855925.974933839</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>135</v>
+      </c>
+      <c r="B129" t="n">
+        <v>841239.168907487</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>136</v>
+      </c>
+      <c r="B130" t="n">
+        <v>965084.02143623</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>137</v>
+      </c>
+      <c r="B131" t="n">
+        <v>991554.158700586</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>138</v>
+      </c>
+      <c r="B132" t="n">
+        <v>861034.052974877</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>139</v>
+      </c>
+      <c r="B133" t="n">
+        <v>846833.361163838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>